<commit_message>
Related companies is working
</commit_message>
<xml_diff>
--- a/empresas_info.xlsx
+++ b/empresas_info.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
   <si>
     <t>Empresa buscada</t>
   </si>
@@ -53,6 +53,147 @@
   </si>
   <si>
     <t>Ayuntamiento</t>
+  </si>
+  <si>
+    <t>Relacionado (Cascante)</t>
+  </si>
+  <si>
+    <t>Inyecciones Plásticas Mecacontrol</t>
+  </si>
+  <si>
+    <t>Carr. Tudela - Tarazona, 10, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 84 45 21</t>
+  </si>
+  <si>
+    <t>http://www.inyeccionesmecacontrol.com/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Inyecciones+Pl%C3%A1sticas+Mecacontrol/@41.9894472,-1.6827796,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a51fdf53dea27:0x9823af5de2de00a8!8m2!3d41.9894472!4d-1.6782735!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhkgEhcGxhc3RpY19pbmplY3Rpb25fbW9sZGluZ19zZXJ2aWNlqgFUEAEqDCIIZW1wcmVzYXMoDjIgEAEiHPN-cHidLlggMybfITUEhVsbNWgSxpnAvZ-OxigyIBACIhxlbXByZXNhcyBlbiBjYXNjYW50ZSBlc3Bhw7Fh4AEA!16s%2Fg%2F1q5bnr7lf?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Empresa de moldeo por inyección de plástico</t>
+  </si>
+  <si>
+    <t>Vibracoustic Cascante</t>
+  </si>
+  <si>
+    <t>Ctra. Tudela-Tarazona, s/n, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 84 45 06</t>
+  </si>
+  <si>
+    <t>https://www.vibracoustic.com/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Vibracoustic+Cascante/@41.9894472,-1.6827796,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a51fe3f7664cb:0xf61aec36796f3de!8m2!3d41.990382!4d-1.6777962!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhkgEXYXV0b19wYXJ0c19tYW51ZmFjdHVyZXKqAVQQASoMIghlbXByZXNhcygOMiAQASIc835weJ0uWCAzJt8hNQSFWxs1aBLGmcC9n47GKDIgEAIiHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWHgAQA!16s%2Fg%2F1trszbgr?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Fabricante de repuestos para automóviles</t>
+  </si>
+  <si>
+    <t>Industrias Areso</t>
+  </si>
+  <si>
+    <t>Pol. Industrial El Parral, Nave 8-9, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 85 15 52</t>
+  </si>
+  <si>
+    <t>http://www.aresoguantes.com/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Industrias+Areso/@41.9894472,-1.6827796,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a51fdf53dea27:0x45792b426f5264cd!8m2!3d41.9917081!4d-1.6776739!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhWh4iHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWGSARxwcm90ZWN0aXZlX2Nsb3RoaW5nX3N1cHBsaWVymgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU4yY0hGRFdEUkJSUkFCqgFUEAEqDCIIZW1wcmVzYXMoDjIgEAEiHPN-cHidLlggMybfITUEhVsbNWgSxpnAvZ-OxigyIBACIhxlbXByZXNhcyBlbiBjYXNjYW50ZSBlc3Bhw7Fh4AEA-gEECAAQOw!16s%2Fg%2F12qghm7tl?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Edmar S A</t>
+  </si>
+  <si>
+    <t>Carr. Tudela - Tarazona, 23, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 85 02 83</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Edmar+S+A/@41.9962921,-1.6788175,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a4e02ce7d0713:0xa533a4393fce17f3!8m2!3d41.9962921!4d-1.6743114!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhkgEdaW5kdXN0cmlhbF9lcXVpcG1lbnRfc3VwcGxpZXKqAVQQASoMIghlbXByZXNhcygOMiAQASIc835weJ0uWCAzJt8hNQSFWxs1aBLGmcC9n47GKDIgEAIiHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWHgAQA!16s%2Fg%2F1z44b4sz9?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Empresa de suministros industriales</t>
+  </si>
+  <si>
+    <t>Galipienzo</t>
+  </si>
+  <si>
+    <t>C. Vía Romana, 0, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 85 16 66</t>
+  </si>
+  <si>
+    <t>https://galipienzo.es/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Galipienzo/@42.0107959,-1.6882863,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a51e23bf46c7f:0xfb0b0ad90ea41d5e!8m2!3d42.0107959!4d-1.6837802!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhkgEOc2xhdWdodGVyaG91c2WqAVQQASoMIghlbXByZXNhcygOMiAQASIc835weJ0uWCAzJt8hNQSFWxs1aBLGmcC9n47GKDIgEAIiHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWHgAQA!16s%2Fg%2F12qggw6dh?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Matadero</t>
+  </si>
+  <si>
+    <t>Bodegas Malón de Echaide</t>
+  </si>
+  <si>
+    <t>Carr. Tudela - Tarazona, 33, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 85 14 11</t>
+  </si>
+  <si>
+    <t>http://www.malondeechaide.com/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Bodegas+Mal%C3%B3n+de+Echaide/@41.9937281,-1.679878,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a4e029a58e90f:0x6b8273c2b56a20b5!8m2!3d41.9937281!4d-1.6753719!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhWh4iHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWGSAQZ3aW5lcnmaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVUmlhR05FYkdsUlJSQUKqAVQQASoMIghlbXByZXNhcygOMiAQASIc835weJ0uWCAzJt8hNQSFWxs1aBLGmcC9n47GKDIgEAIiHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWHgAQD6AQUIlgIQEg!16s%2Fg%2F1tdc6kj8?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Bodega</t>
+  </si>
+  <si>
+    <t>Centro Termolúdico Cascante</t>
+  </si>
+  <si>
+    <t>C. Fundacion Fuentes Dutor, s/n, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 84 45 38</t>
+  </si>
+  <si>
+    <t>http://www.termoludicocascante.es/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Centro+Termol%C3%BAdico+Cascante/@41.9931,-1.6918171,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a51f06019eabf:0xa4ee85a48f3119fc!8m2!3d41.9931!4d-1.687311!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhWh4iHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWGSARNzcGFfYW5kX2hlYWx0aF9jbHVimgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVVIxYVdWbWJ6ZEJSUkFCqgFUEAEqDCIIZW1wcmVzYXMoDjIgEAEiHPN-cHidLlggMybfITUEhVsbNWgSxpnAvZ-OxigyIBACIhxlbXByZXNhcyBlbiBjYXNjYW50ZSBlc3Bhw7Fh4AEA-gEECAsQRg!16s%2Fg%2F1v_z5nbn?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Spa y gimnasio</t>
+  </si>
+  <si>
+    <t>EADEC · Etiquetas Adhesivas Ecológicas</t>
+  </si>
+  <si>
+    <t>Polígono el Parral, 5, 31520 Cascante, Navarra, España</t>
+  </si>
+  <si>
+    <t>+34 948 85 08 35</t>
+  </si>
+  <si>
+    <t>https://eadec.es/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/EADEC+%C2%B7+Etiquetas+Adhesivas+Ecol%C3%B3gicas/@41.9908239,-1.6824224,17z/data=!4m10!1m2!2m1!1sEmpresas+en+Cascante+Espa%C3%B1a!3m6!1s0xd5a4e027ecb5463:0xfcb68d187c69f39c!8m2!3d41.9908239!4d-1.6779163!15sChxFbXByZXNhcyBlbiBDYXNjYW50ZSBFc3Bhw7FhWh4iHGVtcHJlc2FzIGVuIGNhc2NhbnRlIGVzcGHDsWGSARRzdGlja2VyX21hbnVmYWN0dXJlcqoBVBABKgwiCGVtcHJlc2FzKA4yIBABIhzzfnB4nS5YIDMm3yE1BIVbGzVoEsaZwL2fjsYoMiAQAiIcZW1wcmVzYXMgZW4gY2FzY2FudGUgZXNwYcOxYeABAA!16s%2Fg%2F1tgzcp6s?entry=ttu&amp;g_ep=EgoyMDI1MDYwNC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>Impresora de etiquetas personalizadas</t>
   </si>
   <si>
     <t>Panadería Celia</t>
@@ -101,12 +242,17 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCE5FF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,8 +267,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
@@ -520,49 +667,233 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>